<commit_message>
Add authentication error handling
</commit_message>
<xml_diff>
--- a/server/routes/student-workbook.xlsx
+++ b/server/routes/student-workbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Фамилия Имя</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>Котусев Дмитрий</t>
+  </si>
+  <si>
+    <t>123 123</t>
+  </si>
+  <si>
+    <t>BSU</t>
+  </si>
+  <si>
+    <t>A1</t>
   </si>
 </sst>
 </file>
@@ -693,6 +702,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>2023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>